<commit_message>
fill new execution metrics for configuration 11
</commit_message>
<xml_diff>
--- a/test-code-generator/Evaluation/QuantitativeEvaluation/11/others/UC3.2_TC1.xlsx
+++ b/test-code-generator/Evaluation/QuantitativeEvaluation/11/others/UC3.2_TC1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\Università\Tesi magistrale\Evaluation\QuantitativeEvaluation_NewGenerated\9\others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sronz\Documents\GitHub\LLM-based-UCTframework\test-code-generator\Evaluation\QuantitativeEvaluation\11\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F408CC45-68DC-47FD-8FF4-96B070B49B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DB1A3-A3A2-455A-95FB-707F9EBEFD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2436" yWindow="480" windowWidth="18684" windowHeight="11448" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuantitativeMetrics" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -151,7 +151,10 @@
     <t>UC3.2_TC1</t>
   </si>
   <si>
-    <t>Missing import in .functions.js</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>invalid expect</t>
   </si>
 </sst>
 </file>
@@ -575,11 +578,9 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
@@ -588,7 +589,9 @@
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
         <v>34</v>
@@ -598,8 +601,12 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -780,6 +787,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f30c6ab7-8926-430d-82bc-5e99a9f1e9d8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="856457a6-4dfa-4794-b0af-7f9bf7b747ed">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006787F7477D2EAB4386C2F3BB056A2A76" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="96c5202f1ec23b58096e9092aca08dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="856457a6-4dfa-4794-b0af-7f9bf7b747ed" xmlns:ns3="f30c6ab7-8926-430d-82bc-5e99a9f1e9d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa211f3d89e43681eb2a30aba4fe6d4f" ns2:_="" ns3:_="">
     <xsd:import namespace="856457a6-4dfa-4794-b0af-7f9bf7b747ed"/>
@@ -974,27 +1001,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f30c6ab7-8926-430d-82bc-5e99a9f1e9d8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="856457a6-4dfa-4794-b0af-7f9bf7b747ed">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584F92B2-20EF-480D-96FA-E87137FBBCB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D44E722F-21C5-4BAF-9B32-B2E5E93B716E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f30c6ab7-8926-430d-82bc-5e99a9f1e9d8"/>
+    <ds:schemaRef ds:uri="856457a6-4dfa-4794-b0af-7f9bf7b747ed"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F098DE97-9011-442D-BD45-7972233C6879}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1011,23 +1037,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D44E722F-21C5-4BAF-9B32-B2E5E93B716E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f30c6ab7-8926-430d-82bc-5e99a9f1e9d8"/>
-    <ds:schemaRef ds:uri="856457a6-4dfa-4794-b0af-7f9bf7b747ed"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584F92B2-20EF-480D-96FA-E87137FBBCB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>